<commit_message>
Allows missing links between neurons of neighbor tiers
</commit_message>
<xml_diff>
--- a/src/test/resources/test_model_real.xlsx
+++ b/src/test/resources/test_model_real.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sources\neural_network\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DC5C25-85FC-4307-8667-1CBD252479D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B435364B-B78A-46EA-885E-0C7C97FE8C3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EFCF6C60-05F7-44DB-8BA7-596D5CCBC49A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EFCF6C60-05F7-44DB-8BA7-596D5CCBC49A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="5">
   <si>
     <t>pseudo()</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>lin(0.7)</t>
+  </si>
+  <si>
+    <t>sig(0.4)</t>
+  </si>
+  <si>
+    <t>sig(0.8)</t>
   </si>
 </sst>
 </file>
@@ -397,15 +403,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81C2F759-7B1A-49DF-B2D4-12EDF5D848B6}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -426,7 +432,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,10 +490,10 @@
         <v>0</v>
       </c>
       <c r="Q1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -581,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B48C614-211A-4145-8C99-B15EF6D0DCEC}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refactoring of the dataSets
</commit_message>
<xml_diff>
--- a/src/test/resources/test_model_real.xlsx
+++ b/src/test/resources/test_model_real.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sources\neural_network\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B435364B-B78A-46EA-885E-0C7C97FE8C3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE65657-AB18-45A1-BEF5-D366FA1349BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EFCF6C60-05F7-44DB-8BA7-596D5CCBC49A}"/>
   </bookViews>
@@ -34,12 +34,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="6">
   <si>
     <t>pseudo()</t>
-  </si>
-  <si>
-    <t>sig(0.9)</t>
   </si>
   <si>
     <t>lin(0.7)</t>
@@ -49,6 +46,12 @@
   </si>
   <si>
     <t>sig(0.8)</t>
+  </si>
+  <si>
+    <t>sig(0.90)</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -490,10 +493,10 @@
         <v>0</v>
       </c>
       <c r="Q1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R1" t="s">
         <v>3</v>
-      </c>
-      <c r="R1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -585,10 +588,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B48C614-211A-4145-8C99-B15EF6D0DCEC}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,111 +610,597 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.5</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
       <c r="B3">
         <v>0.5</v>
       </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
       <c r="C4">
         <v>0.5</v>
       </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
       <c r="E5">
         <v>0.5</v>
       </c>
+      <c r="F5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
       <c r="D6">
         <v>0.5</v>
       </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
       <c r="E7">
         <v>0.5</v>
       </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G9">
-        <v>0.5</v>
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>0.5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F10">
-        <v>0.5</v>
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>0.5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G11">
-        <v>0.5</v>
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>0.5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H12">
-        <v>0.5</v>
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>0.5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" t="s">
+        <v>5</v>
+      </c>
+      <c r="J12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F13">
-        <v>0.5</v>
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>0.5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J13" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G14">
-        <v>0.5</v>
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>0.5</v>
+      </c>
+      <c r="I14" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H15">
-        <v>0.5</v>
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>0.5</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F16">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G17">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="18" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="H18">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="19" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="I19">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="J20">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16">
+        <v>0.5</v>
+      </c>
+      <c r="H16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>5</v>
+      </c>
+      <c r="J16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>0.5</v>
+      </c>
+      <c r="I17" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>0.5</v>
+      </c>
+      <c r="J18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19">
         <v>0.5</v>
       </c>
     </row>
@@ -732,7 +1221,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>